<commit_message>
Updated readme and ordering info
</commit_message>
<xml_diff>
--- a/Util/Ordering Info/AutoPowerBoxTesterv1.1/AssemblyFiles/BOM.xlsx
+++ b/Util/Ordering Info/AutoPowerBoxTesterv1.1/AssemblyFiles/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernardo.Perez\ArduinoSketchbook\Arduino-Power-Box-Tester\util\Ordering Info\AutoPowerBoxTesterv1.1\AssemblyFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDADA1C-1F38-4C8F-AE3B-15BA98B4DD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A1E54A-775C-445B-9A12-5DD40F2C369E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7708390F-2016-49A3-B238-8E28142561CF}"/>
+    <workbookView xWindow="-28920" yWindow="-11250" windowWidth="29040" windowHeight="15840" xr2:uid="{7708390F-2016-49A3-B238-8E28142561CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="87">
   <si>
     <t>Description</t>
   </si>
@@ -290,6 +290,12 @@
   </si>
   <si>
     <t>CON_430450212</t>
+  </si>
+  <si>
+    <t>RMCF2512FT100K</t>
+  </si>
+  <si>
+    <t>1206YC204KAT4A</t>
   </si>
 </sst>
 </file>
@@ -665,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16AA6FF-6C0B-4447-9390-74E0640C9AA6}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -774,6 +780,9 @@
       <c r="B6">
         <v>2</v>
       </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
       <c r="D6" t="s">
         <v>47</v>
       </c>
@@ -788,6 +797,9 @@
       <c r="B7">
         <v>2</v>
       </c>
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
       <c r="D7" t="s">
         <v>44</v>
       </c>
@@ -854,7 +866,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>39293083</v>
+        <v>39281083</v>
       </c>
       <c r="D11" t="s">
         <v>54</v>

</xml_diff>